<commit_message>
Parallel and CrossBrowser Testing added
</commit_message>
<xml_diff>
--- a/Selenium/src/main/resources/Test_Data.xlsx
+++ b/Selenium/src/main/resources/Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Demo Web Shop</t>
-  </si>
-  <si>
-    <t>Good</t>
   </si>
   <si>
     <t>abctest439@gmail.com</t>
@@ -55,6 +52,12 @@
       </rPr>
       <t>d</t>
     </r>
+  </si>
+  <si>
+    <t>Test123</t>
+  </si>
+  <si>
+    <t>Poor</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -417,7 +422,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -428,10 +433,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,25 +444,34 @@
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="D1" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -465,7 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -477,10 +491,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>